<commit_message>
Re-TL S00100, S00101 (opening scene)
</commit_message>
<xml_diff>
--- a/tl/S00100.MES.BIN.xlsx
+++ b/tl/S00100.MES.BIN.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19512109-5D7D-438F-9DBC-D5D85CA45056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C0BB25-1C0E-42DB-8DB7-61E31543BE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="11310" windowWidth="48240" windowHeight="19545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1530" yWindow="18150" windowWidth="55185" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00100.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="282">
   <si>
     <t>Status</t>
   </si>
@@ -50,30 +50,45 @@
     <t>1</t>
   </si>
   <si>
+    <t>…Starting from today, my new life in this new room begins.</t>
+  </si>
+  <si>
     <t>...Well, from today on, my new life in this new room begins.</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
+    <t>I should be able to finish tidying up the unpacked boxes from the move soon.</t>
+  </si>
+  <si>
     <t>I'll finish unpacking the moving boxes in a little while too.</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>It's totally unreasonable that I have to move during my first year of college in the autumn just because of my parents' whim.</t>
+  </si>
+  <si>
     <t>It's totally unreasonable for my parents to make me move in the middle of my first year in college.</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
+    <t>Oh well, let's just get it over with as soon as possible.</t>
+  </si>
+  <si>
     <t>Oh well, I'll just get it over with quickly.</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
+    <t>Ding---dong.</t>
+  </si>
+  <si>
     <t>Ding-dong.</t>
   </si>
   <si>
@@ -86,6 +101,9 @@
     <t>13</t>
   </si>
   <si>
+    <t>My room is a total mess, though.</t>
+  </si>
+  <si>
     <t>The room is a mess though.</t>
   </si>
   <si>
@@ -101,12 +119,18 @@
     <t>17</t>
   </si>
   <si>
+    <t>I reply and head towards the front door.</t>
+  </si>
+  <si>
     <t>I reply and head to the front door.</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
+    <t>Who could it be…?</t>
+  </si>
+  <si>
     <t>Who could it be...?</t>
   </si>
   <si>
@@ -119,30 +143,45 @@
     <t>Yuki</t>
   </si>
   <si>
+    <t>Good morning, Touya-kun…</t>
+  </si>
+  <si>
     <t>"Good morning, Touya-kun..."</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
+    <t>Oh, Yuki.</t>
+  </si>
+  <si>
     <t>"Oh, Yuki."</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
+    <t>Um... I have something I want to talk to you about... Is now okay?</t>
+  </si>
+  <si>
     <t>I have something I want to talk to you about... is now okay?</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
+    <t>Eh? Ah, sure…</t>
+  </si>
+  <si>
     <t>"What? Oh, in that case..."</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
+    <t>Come in. …It's a mess, though.</t>
+  </si>
+  <si>
     <t>Come in. It's a bit messy in here though.</t>
   </si>
   <si>
@@ -155,15 +194,24 @@
     <t>33</t>
   </si>
   <si>
+    <t>The girl smiling gently at me is Yuki Morikawa.</t>
+  </si>
+  <si>
     <t>The girl smiling gently at me is Morikawa Yuki.</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
+    <t>…She's my girlfriend.</t>
+  </si>
+  <si>
     <t>... She's my girlfriend.</t>
   </si>
   <si>
+    <t>Add "she's"</t>
+  </si>
+  <si>
     <t>37</t>
   </si>
   <si>
@@ -173,78 +221,120 @@
     <t>39</t>
   </si>
   <si>
+    <t>We often showed each other our textbooks and homework, and talked about random things together.</t>
+  </si>
+  <si>
     <t>We often showed each other our textbooks and homework and had idle conversations.</t>
   </si>
   <si>
     <t>41</t>
   </si>
   <si>
+    <t>I think that close physical distance made us feel close to each other's hearts.</t>
+  </si>
+  <si>
     <t>I think the close proximity made us feel close to each other.</t>
   </si>
   <si>
     <t>43</t>
   </si>
   <si>
+    <t>Around that time, Yuki was attending singing school, and would go home immediately after classes ended.</t>
+  </si>
+  <si>
     <t>Around that time, it seemed like Yuki was attending a training school for singers and would go home immediately after class ended.</t>
   </si>
   <si>
+    <t>Drop "it seemed"</t>
+  </si>
+  <si>
     <t>45</t>
   </si>
   <si>
+    <t>…She was a beautiful girl even within in the school, but her 'poor social skills' kept the boys in school from making advances towards her.</t>
+  </si>
+  <si>
     <t>...She was a beautiful person at school, but her "difficulty in maintaining relationships" might have been the reason why male students at school kept their distance from her.</t>
   </si>
   <si>
     <t>47</t>
   </si>
   <si>
+    <t>As for why she and I became lovers…</t>
+  </si>
+  <si>
     <t>As for how I managed to become lovers with such a girl...</t>
   </si>
   <si>
     <t>49</t>
   </si>
   <si>
+    <t>I think it was on the way home from school.</t>
+  </si>
+  <si>
     <t>After school, I think I was on my way home.</t>
   </si>
   <si>
     <t>51</t>
   </si>
   <si>
+    <t>By chance, we happened to be walking together, side-by-side, when Yuki suddenly stopped.</t>
+  </si>
+  <si>
     <t>We happened to be together and were walking side by side when Yuki suddenly stopped.</t>
   </si>
   <si>
     <t>53</t>
   </si>
   <si>
+    <t>What's wrong?</t>
+  </si>
+  <si>
     <t>Is something wrong?</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
+    <t>It's nothing, but…</t>
+  </si>
+  <si>
     <t>It's nothing, but...</t>
   </si>
   <si>
     <t>57</t>
   </si>
   <si>
+    <t>Yuki looked around the area like she was seeing it for the first time, and said softly,</t>
+  </si>
+  <si>
     <t>Like we were on a road we've never walked on before, Yuki quietly looked around and spoke.</t>
   </si>
   <si>
     <t>59</t>
   </si>
   <si>
+    <t>It feels strange, doesn't it?</t>
+  </si>
+  <si>
     <t>It feels strange.</t>
   </si>
   <si>
     <t>61</t>
   </si>
   <si>
+    <t>Huh?</t>
+  </si>
+  <si>
     <t>What?</t>
   </si>
   <si>
     <t>63</t>
   </si>
   <si>
+    <t>I talk to you a lot, Fujii-kun, but this is the first time we're walking home together.</t>
+  </si>
+  <si>
     <t>I talk to you a lot, Fuji-kun, but this is the first time we're walking home together.</t>
   </si>
   <si>
@@ -257,102 +347,114 @@
     <t>67</t>
   </si>
   <si>
+    <t>At that time, we weren't that close yet, and we didn't talk as much as we were just friendly with each other.</t>
+  </si>
+  <si>
     <t>We weren't that close at the time, and we didn't really talk that much.</t>
   </si>
   <si>
     <t>69</t>
   </si>
   <si>
+    <t>But, it wasn't like I was completely unaware of her….</t>
+  </si>
+  <si>
     <t>But, it's not like I wasn't aware of it either...</t>
   </si>
   <si>
-    <t>But, it's not like I wasn't aware of it...</t>
-  </si>
-  <si>
     <t>71</t>
   </si>
   <si>
+    <t>I also thought it felt as if we were a bit like lovers, or something.</t>
+  </si>
+  <si>
     <t>I also thought we were just a little bit like lovers, or something.</t>
   </si>
   <si>
-    <t>I also thought we were like lovers, or something, just a little.</t>
-  </si>
-  <si>
     <t>73</t>
   </si>
   <si>
+    <t>I meant it as a joke, as an extension of our usual conversation.</t>
+  </si>
+  <si>
     <t>I meant it as a joke, like an extension of our usual conversation.</t>
   </si>
   <si>
     <t>75</t>
   </si>
   <si>
+    <t>But after that, the conversation came to a halt.</t>
+  </si>
+  <si>
     <t>But after that, the conversation stopped.</t>
   </si>
   <si>
     <t>77</t>
   </si>
   <si>
+    <t>I was looking at Yuki's fingertips, which were aligned with the handle of her school bag.</t>
+  </si>
+  <si>
     <t>I was looking at the tips of Yuki's fingers, which were wrapped around the handle of her school bag.</t>
   </si>
   <si>
-    <t>I was looking at the tips of Yuki's fingers, arranged on the handle of my school bag.</t>
-  </si>
-  <si>
     <t>79</t>
   </si>
   <si>
+    <t>They were beautiful, slender fingers, I thought to myself.</t>
+  </si>
+  <si>
     <t>They were beautiful, delicate fingers, I thought.</t>
   </si>
   <si>
-    <t>They were beautiful, I thought they were delicate fingers.</t>
-  </si>
-  <si>
     <t>81</t>
   </si>
   <si>
+    <t>At that moment, I noticed Yuki suddenly took a deep breath.</t>
+  </si>
+  <si>
     <t>At that moment, I noticed Yuki took a deep breath.</t>
   </si>
   <si>
-    <t>At that moment, I noticed Yuki took a deep breath, like she had made a big decision.</t>
-  </si>
-  <si>
     <t>83</t>
   </si>
   <si>
+    <t>As if she had just made an important decision.</t>
+  </si>
+  <si>
     <t>She looked like she had made a big decision.</t>
   </si>
   <si>
     <t>85</t>
   </si>
   <si>
+    <t>You know, all this time…</t>
+  </si>
+  <si>
     <t>A little bit...</t>
   </si>
   <si>
-    <t>I've liked you for a long time... -- The voice line says "chotto ne", so she's reciting Touya's "little bit" line.</t>
-  </si>
-  <si>
     <t>87</t>
   </si>
   <si>
+    <t>And then, Yuki said,</t>
+  </si>
+  <si>
     <t>And then she said.</t>
   </si>
   <si>
-    <t>"And then, Yuki said."</t>
-  </si>
-  <si>
     <t>89</t>
   </si>
   <si>
     <t>Fujii-kun, I've liked you for a long time now.</t>
   </si>
   <si>
-    <t>Fujii-kun, I've liked you for a while now.'"</t>
-  </si>
-  <si>
     <t>91</t>
   </si>
   <si>
+    <t>Um…</t>
+  </si>
+  <si>
     <t>Um...</t>
   </si>
   <si>
@@ -365,45 +467,57 @@
     <t>95</t>
   </si>
   <si>
+    <t>She smiled awkwardly.</t>
+  </si>
+  <si>
     <t>She laughed awkwardly.</t>
   </si>
   <si>
     <t>97</t>
   </si>
   <si>
+    <t>To be honest, I had been quite interested in Yuki as well.</t>
+  </si>
+  <si>
     <t>To tell the truth, I had been quite interested in Yuki as well.</t>
   </si>
   <si>
     <t>99</t>
   </si>
   <si>
+    <t>That's why I answered right away.</t>
+  </si>
+  <si>
     <t>So, I answered right away.</t>
   </si>
   <si>
     <t>101</t>
   </si>
   <si>
+    <t>I liked you too, though…</t>
+  </si>
+  <si>
     <t>I liked you too, but...</t>
   </si>
   <si>
     <t>103</t>
   </si>
   <si>
+    <t>I couldn't find any words to say after that.</t>
+  </si>
+  <si>
     <t>After that, there were no more words.</t>
   </si>
   <si>
-    <t>After that, there are no more words.</t>
-  </si>
-  <si>
     <t>105</t>
   </si>
   <si>
+    <t>Again, the conversation stopped for a while.</t>
+  </si>
+  <si>
     <t>Again, for a little while, it was silent.</t>
   </si>
   <si>
-    <t>Again, for a little while, words are cut off.</t>
-  </si>
-  <si>
     <t>107</t>
   </si>
   <si>
@@ -413,40 +527,52 @@
     <t>109</t>
   </si>
   <si>
+    <t>Yuki said that.</t>
+  </si>
+  <si>
     <t>Yuki said.</t>
   </si>
   <si>
     <t>111</t>
   </si>
   <si>
+    <t>Then, let's use the present tense from here on out.</t>
+  </si>
+  <si>
     <t>Then, from here on out, let's use the present tense.</t>
   </si>
   <si>
     <t>113</t>
   </si>
   <si>
+    <t>Yuki nodded slightly in response to my answer.</t>
+  </si>
+  <si>
     <t>When I answered, Yuki nodded slightly.</t>
   </si>
   <si>
-    <t>When I answered, Yuki nodded just a little bit.</t>
-  </si>
-  <si>
     <t>115</t>
   </si>
   <si>
+    <t>After that, we both blushed.</t>
+  </si>
+  <si>
     <t>After that, the two of us got embarrassed.</t>
   </si>
   <si>
-    <t>Same but modified for past-tense since it's during a flashback</t>
+    <t>Change to blushed</t>
   </si>
   <si>
     <t>117</t>
   </si>
   <si>
+    <t>And like that, we probably became lovers….</t>
+  </si>
+  <si>
     <t>I guess that made us become lovers.</t>
   </si>
   <si>
-    <t>That's how it was, we probably became lovers...</t>
+    <t>This line is so hard to translate! The literal translation is very awkward because of 多分</t>
   </si>
   <si>
     <t>119</t>
@@ -455,24 +581,24 @@
     <t>Fufufu. What's wrong? How come you're quiet all of a sudden?</t>
   </si>
   <si>
-    <t>Fufufu. What's wrong? Suddenly so quiet?</t>
-  </si>
-  <si>
     <t>121</t>
   </si>
   <si>
+    <t>Eh? Ahh, it's nothing…</t>
+  </si>
+  <si>
     <t>Huh? Oh, no...</t>
   </si>
   <si>
     <t>123</t>
   </si>
   <si>
+    <t>After graduating from high school, Yuki and I enrolled in the same university.</t>
+  </si>
+  <si>
     <t>After graduating high school, Yuki and I enrolled in the same university.</t>
   </si>
   <si>
-    <t>After graduating high school, Yuki and I went to the same university.</t>
-  </si>
-  <si>
     <t>125</t>
   </si>
   <si>
@@ -482,27 +608,36 @@
     <t>127</t>
   </si>
   <si>
+    <t>Sometimes, I think Yuki is the ideal partner.</t>
+  </si>
+  <si>
     <t>Sometimes I think Yuki is the ideal partner.</t>
   </si>
   <si>
     <t>129</t>
   </si>
   <si>
+    <t>Of course she's cute, but there's something about her that makes her fun to be around, and she always tries to be by my side.</t>
+  </si>
+  <si>
     <t>Of course she's cute, but it's also fun to be with her. Furthermore, she tries to be by my side even if I'm not thinking about wanting to be by hers.</t>
   </si>
   <si>
-    <t>Of course she's cute to look at, but it's fun to be with her, and furthermore, she tries to be by my side even if I'm not thinking about wanting to be by her side.</t>
-  </si>
-  <si>
     <t>131</t>
   </si>
   <si>
+    <t>I feel like, even more than me wanting to be by her side, she wants to be by mine, and even though it's just a feeling, I'm certain of it….</t>
+  </si>
+  <si>
     <t>I feel vaguely certain that she wants to be by my side, more than I want to be by hers...</t>
   </si>
   <si>
     <t>133</t>
   </si>
   <si>
+    <t>Ah, but more importantly, what did you want to talk about? …all of a sudden?</t>
+  </si>
+  <si>
     <t>Oh, but more importantly, what's this about a conversation? ...all of a sudden?</t>
   </si>
   <si>
@@ -515,141 +650,192 @@
     <t>137</t>
   </si>
   <si>
+    <t>Even though we can meet whenever since starting university.</t>
+  </si>
+  <si>
     <t>Even though we can see each other after university starts.</t>
   </si>
   <si>
-    <t>Even though we can see each other since starting university.</t>
-  </si>
-  <si>
     <t>139</t>
   </si>
   <si>
+    <t>Yeah…. The thing is…</t>
+  </si>
+  <si>
     <t>Yeah... Um, well...</t>
   </si>
   <si>
     <t>141</t>
   </si>
   <si>
+    <t>…Um, I've decided to make my debut…</t>
+  </si>
+  <si>
     <t>...Um, I, well, I'm going to debut...</t>
   </si>
   <si>
     <t>143</t>
   </si>
   <si>
+    <t>Huh…?</t>
+  </si>
+  <si>
     <t>Huh...?</t>
   </si>
   <si>
     <t>145</t>
   </si>
   <si>
+    <t>Do you know of Eiji Ogata? Of Ogata Productions. He's the one who debuted Rina Ogata.</t>
+  </si>
+  <si>
     <t>Do you know Eiji Ogata? Of Ogata Productions. He's the one who debuted Rina Ogata.</t>
   </si>
   <si>
     <t>147</t>
   </si>
   <si>
+    <t>Y-yeah…</t>
+  </si>
+  <si>
     <t>Oh, yeah...</t>
   </si>
   <si>
     <t>149</t>
   </si>
   <si>
+    <t>So, I've decided to make my debut with his help…</t>
+  </si>
+  <si>
     <t>From there, I've decided to debut under Mr. Ogata's production...</t>
   </si>
   <si>
     <t>151</t>
   </si>
   <si>
+    <t>Really…?</t>
+  </si>
+  <si>
     <t>Really...?</t>
   </si>
   <si>
     <t>153</t>
   </si>
   <si>
+    <t>Yeah…</t>
+  </si>
+  <si>
     <t>Yeah...</t>
   </si>
   <si>
     <t>155</t>
   </si>
   <si>
+    <t>Amazing…! That's amazing, Yuki!!</t>
+  </si>
+  <si>
     <t>That's amazing! That's amazing, Yuki!!</t>
   </si>
   <si>
     <t>157</t>
   </si>
   <si>
+    <t>…But, Yuki doesn't seem as excited as me….</t>
+  </si>
+  <si>
     <t>...but, Yuki doesn't seem as excited as me...</t>
   </si>
   <si>
-    <t>...but, Yuki, doesn't seem as excited as me...</t>
-  </si>
-  <si>
     <t>159</t>
   </si>
   <si>
+    <t>But, you know… …That's why, we might not be able to spend as much time together as before…</t>
+  </si>
+  <si>
     <t>But you know... ...that's why, from now on, there might not be much time for us to be together...</t>
   </si>
   <si>
-    <t>But you see... ...so, from now on, there might not be much time for us to be together...</t>
-  </si>
-  <si>
     <t>161</t>
   </si>
   <si>
+    <t>Ah…</t>
+  </si>
+  <si>
     <t>Ah...</t>
   </si>
   <si>
     <t>163</t>
   </si>
   <si>
+    <t>So that's it….</t>
+  </si>
+  <si>
     <t>So that's it...</t>
   </si>
   <si>
     <t>165</t>
   </si>
   <si>
+    <t>"My Yuki" is going to disappear…?</t>
+  </si>
+  <si>
     <t>"My Yuki" is going to disappear?</t>
   </si>
   <si>
     <t>167</t>
   </si>
   <si>
+    <t>But, you have to do your best. …after all, you've worked really hard for this, Yuki.</t>
+  </si>
+  <si>
     <t>But, you have to do your best. ...after all, Yuki, you've been working hard for this...</t>
   </si>
   <si>
-    <t>But, we have to do our best. ...after all, Yuki has been working hard for this...</t>
-  </si>
-  <si>
     <t>169</t>
   </si>
   <si>
     <t>171</t>
   </si>
   <si>
+    <t>I can't say that I won't feel lonely either…</t>
+  </si>
+  <si>
     <t>I'm not going to be completely lonely, but...</t>
   </si>
   <si>
     <t>173</t>
   </si>
   <si>
+    <t>But….</t>
+  </si>
+  <si>
     <t>but...</t>
   </si>
   <si>
     <t>175</t>
   </si>
   <si>
+    <t>But, do your best. I'll be cheering you on.</t>
+  </si>
+  <si>
     <t>But, do your best. I'll cheer you on.</t>
   </si>
   <si>
     <t>177</t>
   </si>
   <si>
+    <t>But…</t>
+  </si>
+  <si>
     <t>But...</t>
   </si>
   <si>
     <t>179</t>
   </si>
   <si>
+    <t>It's okay. …It might be tough, but let's make our dreams come true together.</t>
+  </si>
+  <si>
     <t>It's okay. ...it might be a little tough, but let's make our dreams come true together.</t>
   </si>
   <si>
@@ -662,19 +848,19 @@
     <t>183</t>
   </si>
   <si>
+    <t>Y-yeah!</t>
+  </si>
+  <si>
     <t>"Y-yeah!"</t>
   </si>
   <si>
-    <t>O-okay!</t>
-  </si>
-  <si>
     <t>185</t>
   </si>
   <si>
+    <t>And then, Yuki smiles.</t>
+  </si>
+  <si>
     <t>And then, she smiled.</t>
-  </si>
-  <si>
-    <t>And then, Yuki smiled.</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1158,7 +1346,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>9</v>
@@ -1175,7 +1363,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
@@ -1187,10 +1375,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>9</v>
@@ -1207,7 +1395,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
@@ -1219,10 +1407,10 @@
         <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>9</v>
@@ -1239,7 +1427,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
@@ -1251,10 +1439,10 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>9</v>
@@ -1271,7 +1459,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -1283,10 +1471,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>9</v>
@@ -1303,7 +1491,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
@@ -1315,10 +1503,10 @@
         <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>9</v>
@@ -1335,7 +1523,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -1347,10 +1535,10 @@
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>9</v>
@@ -1367,22 +1555,22 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>9</v>
@@ -1399,7 +1587,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
@@ -1411,10 +1599,10 @@
         <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>9</v>
@@ -1431,7 +1619,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -1443,10 +1631,10 @@
         <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>9</v>
@@ -1463,22 +1651,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>9</v>
@@ -1495,22 +1683,22 @@
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>9</v>
@@ -1527,22 +1715,22 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>9</v>
@@ -1559,22 +1747,22 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>9</v>
@@ -1591,22 +1779,22 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>9</v>
@@ -1623,22 +1811,22 @@
         <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>9</v>
@@ -1655,7 +1843,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>9</v>
@@ -1667,10 +1855,10 @@
         <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>9</v>
@@ -1687,7 +1875,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -1699,13 +1887,13 @@
         <v>9</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>9</v>
@@ -1719,7 +1907,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>9</v>
@@ -1731,10 +1919,10 @@
         <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>9</v>
@@ -1751,7 +1939,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -1763,10 +1951,10 @@
         <v>9</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>9</v>
@@ -1783,7 +1971,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
@@ -1795,10 +1983,10 @@
         <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>9</v>
@@ -1815,7 +2003,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -1827,13 +2015,13 @@
         <v>9</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>9</v>
@@ -1847,7 +2035,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>9</v>
@@ -1859,10 +2047,10 @@
         <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>9</v>
@@ -1879,7 +2067,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -1891,10 +2079,10 @@
         <v>9</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>9</v>
@@ -1911,7 +2099,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>9</v>
@@ -1923,10 +2111,10 @@
         <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>9</v>
@@ -1943,7 +2131,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -1955,10 +2143,10 @@
         <v>9</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>9</v>
@@ -1975,22 +2163,22 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>9</v>
@@ -2007,22 +2195,22 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>9</v>
@@ -2039,7 +2227,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
@@ -2051,10 +2239,10 @@
         <v>9</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>9</v>
@@ -2071,22 +2259,22 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>9</v>
@@ -2103,22 +2291,22 @@
         <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>9</v>
@@ -2135,22 +2323,22 @@
         <v>9</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>9</v>
@@ -2167,7 +2355,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
@@ -2179,10 +2367,10 @@
         <v>9</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>9</v>
@@ -2199,7 +2387,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -2211,10 +2399,10 @@
         <v>9</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>9</v>
@@ -2231,7 +2419,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>9</v>
@@ -2243,10 +2431,10 @@
         <v>9</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>9</v>
@@ -2263,22 +2451,22 @@
         <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>9</v>
@@ -2295,7 +2483,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>9</v>
@@ -2307,10 +2495,10 @@
         <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>9</v>
@@ -2327,7 +2515,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
@@ -2339,10 +2527,10 @@
         <v>9</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>9</v>
@@ -2359,7 +2547,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>9</v>
@@ -2371,10 +2559,10 @@
         <v>9</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>9</v>
@@ -2391,7 +2579,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
@@ -2403,10 +2591,10 @@
         <v>9</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>9</v>
@@ -2423,7 +2611,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>9</v>
@@ -2435,10 +2623,10 @@
         <v>9</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>9</v>
@@ -2455,7 +2643,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
@@ -2467,10 +2655,10 @@
         <v>9</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>9</v>
@@ -2487,22 +2675,22 @@
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>9</v>
@@ -2519,7 +2707,7 @@
         <v>9</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
@@ -2531,10 +2719,10 @@
         <v>9</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>9</v>
@@ -2551,22 +2739,22 @@
         <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>9</v>
@@ -2583,22 +2771,22 @@
         <v>9</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>9</v>
@@ -2615,22 +2803,22 @@
         <v>9</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>9</v>
@@ -2647,7 +2835,7 @@
         <v>9</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -2659,10 +2847,10 @@
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>9</v>
+        <v>151</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>9</v>
@@ -2679,7 +2867,7 @@
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>9</v>
@@ -2691,10 +2879,10 @@
         <v>9</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>9</v>
+        <v>154</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>9</v>
@@ -2711,7 +2899,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
@@ -2723,10 +2911,10 @@
         <v>9</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>9</v>
+        <v>157</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>9</v>
@@ -2743,22 +2931,22 @@
         <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>9</v>
@@ -2775,7 +2963,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>9</v>
@@ -2787,10 +2975,10 @@
         <v>9</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>9</v>
@@ -2807,7 +2995,7 @@
         <v>9</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>9</v>
@@ -2819,10 +3007,10 @@
         <v>9</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>9</v>
@@ -2839,22 +3027,22 @@
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>9</v>
@@ -2871,7 +3059,7 @@
         <v>9</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>9</v>
@@ -2883,10 +3071,10 @@
         <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>9</v>
@@ -2903,22 +3091,22 @@
         <v>9</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>9</v>
@@ -2935,7 +3123,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>9</v>
@@ -2947,10 +3135,10 @@
         <v>9</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>9</v>
@@ -2967,7 +3155,7 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>9</v>
@@ -2979,13 +3167,13 @@
         <v>9</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>9</v>
+        <v>181</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>9</v>
@@ -2999,7 +3187,7 @@
         <v>9</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>9</v>
@@ -3011,13 +3199,13 @@
         <v>9</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>9</v>
@@ -3031,22 +3219,22 @@
         <v>9</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>9</v>
@@ -3063,22 +3251,22 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>9</v>
@@ -3095,7 +3283,7 @@
         <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>9</v>
@@ -3107,10 +3295,10 @@
         <v>9</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>9</v>
@@ -3127,7 +3315,7 @@
         <v>9</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>9</v>
@@ -3139,10 +3327,10 @@
         <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>9</v>
+        <v>195</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>9</v>
@@ -3159,7 +3347,7 @@
         <v>9</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>9</v>
@@ -3171,10 +3359,10 @@
         <v>9</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>9</v>
+        <v>198</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>9</v>
@@ -3191,7 +3379,7 @@
         <v>9</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>9</v>
@@ -3203,10 +3391,10 @@
         <v>9</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>9</v>
@@ -3223,7 +3411,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>159</v>
+        <v>202</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>9</v>
@@ -3235,10 +3423,10 @@
         <v>9</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>160</v>
+        <v>203</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>9</v>
+        <v>204</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>9</v>
@@ -3255,22 +3443,22 @@
         <v>9</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>162</v>
+        <v>206</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>9</v>
+        <v>207</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>9</v>
@@ -3287,7 +3475,7 @@
         <v>9</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>163</v>
+        <v>208</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>9</v>
@@ -3299,10 +3487,10 @@
         <v>9</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>9</v>
@@ -3319,7 +3507,7 @@
         <v>9</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>165</v>
+        <v>210</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>9</v>
@@ -3331,10 +3519,10 @@
         <v>9</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>166</v>
+        <v>211</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>167</v>
+        <v>212</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>9</v>
@@ -3351,22 +3539,22 @@
         <v>9</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>9</v>
+        <v>215</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>9</v>
@@ -3383,22 +3571,22 @@
         <v>9</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>170</v>
+        <v>216</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>9</v>
+        <v>218</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>9</v>
@@ -3415,22 +3603,22 @@
         <v>9</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>172</v>
+        <v>219</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>173</v>
+        <v>220</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>9</v>
+        <v>221</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>9</v>
@@ -3447,22 +3635,22 @@
         <v>9</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>9</v>
@@ -3479,22 +3667,22 @@
         <v>9</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>176</v>
+        <v>225</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>177</v>
+        <v>227</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>9</v>
@@ -3511,22 +3699,22 @@
         <v>9</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>9</v>
@@ -3543,22 +3731,22 @@
         <v>9</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>180</v>
+        <v>231</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>181</v>
+        <v>232</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>9</v>
+        <v>233</v>
       </c>
       <c r="H77" s="5" t="s">
         <v>9</v>
@@ -3575,22 +3763,22 @@
         <v>9</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>182</v>
+        <v>234</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>183</v>
+        <v>235</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>9</v>
+        <v>236</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>9</v>
@@ -3607,22 +3795,22 @@
         <v>9</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>184</v>
+        <v>237</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>185</v>
+        <v>238</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>9</v>
+        <v>239</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>9</v>
@@ -3639,7 +3827,7 @@
         <v>9</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>9</v>
@@ -3651,10 +3839,10 @@
         <v>9</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>188</v>
+        <v>242</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>9</v>
@@ -3671,22 +3859,22 @@
         <v>9</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>190</v>
+        <v>244</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>191</v>
+        <v>245</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>9</v>
@@ -3703,22 +3891,22 @@
         <v>9</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>192</v>
+        <v>246</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>193</v>
+        <v>247</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>9</v>
+        <v>248</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>9</v>
@@ -3735,7 +3923,7 @@
         <v>9</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>194</v>
+        <v>249</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>9</v>
@@ -3747,10 +3935,10 @@
         <v>9</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>195</v>
+        <v>250</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>9</v>
+        <v>251</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>9</v>
@@ -3767,7 +3955,7 @@
         <v>9</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>9</v>
@@ -3779,10 +3967,10 @@
         <v>9</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>9</v>
+        <v>254</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>9</v>
@@ -3799,22 +3987,22 @@
         <v>9</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>9</v>
@@ -3831,22 +4019,22 @@
         <v>9</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>201</v>
+        <v>258</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>183</v>
+        <v>235</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>9</v>
+        <v>236</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>9</v>
@@ -3863,7 +4051,7 @@
         <v>9</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>202</v>
+        <v>259</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>9</v>
@@ -3875,10 +4063,10 @@
         <v>9</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>203</v>
+        <v>260</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>9</v>
@@ -3895,7 +4083,7 @@
         <v>9</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>204</v>
+        <v>262</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>9</v>
@@ -3907,10 +4095,10 @@
         <v>9</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>205</v>
+        <v>263</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>9</v>
+        <v>264</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>9</v>
@@ -3927,22 +4115,22 @@
         <v>9</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>206</v>
+        <v>265</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>207</v>
+        <v>266</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>9</v>
+        <v>267</v>
       </c>
       <c r="H89" s="5" t="s">
         <v>9</v>
@@ -3959,22 +4147,22 @@
         <v>9</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>208</v>
+        <v>268</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>9</v>
+        <v>270</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>9</v>
@@ -3991,22 +4179,22 @@
         <v>9</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>210</v>
+        <v>271</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>9</v>
+        <v>273</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>9</v>
@@ -4023,7 +4211,7 @@
         <v>9</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>212</v>
+        <v>274</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>9</v>
@@ -4035,10 +4223,10 @@
         <v>9</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>213</v>
+        <v>275</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>9</v>
+        <v>275</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>9</v>
@@ -4055,22 +4243,22 @@
         <v>9</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>214</v>
+        <v>276</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>216</v>
+        <v>278</v>
       </c>
       <c r="H93" s="5" t="s">
         <v>9</v>
@@ -4087,7 +4275,7 @@
         <v>9</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>217</v>
+        <v>279</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>9</v>
@@ -4099,10 +4287,10 @@
         <v>9</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>218</v>
+        <v>280</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>219</v>
+        <v>281</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>9</v>

</xml_diff>